<commit_message>
Project Case412 is saved. B1 Type: SAVE.
</commit_message>
<xml_diff>
--- a/Case412/module1.xlsx
+++ b/Case412/module1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ekosolapova/work/bugs/TestCasesEPBDS-8483/Case4/Base/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ekosolapova/work/bugs/TestCasesEPBDS-8483/Case4/v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3440347A-CBCA-9846-BE8E-E203C3EC306C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE84CB4-91E9-944E-B032-308A4FAEFBB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11980" yWindow="5900" windowWidth="27640" windowHeight="16940" xr2:uid="{D86F6ED2-5685-5F4F-AC05-266BA9A81085}"/>
   </bookViews>
@@ -75,9 +75,6 @@
     <t>Secondary</t>
   </si>
   <si>
-    <t>Business</t>
-  </si>
-  <si>
     <t>Vacant</t>
   </si>
   <si>
@@ -94,6 +91,9 @@
   </si>
   <si>
     <t>SmartLookup Double Test ( String occupancyType, String policyForm )</t>
+  </si>
+  <si>
+    <t>Business1</t>
   </si>
 </sst>
 </file>
@@ -202,9 +202,6 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -224,6 +221,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -544,7 +544,7 @@
   <dimension ref="E6:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E12" sqref="E12:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -553,108 +553,108 @@
   </cols>
   <sheetData>
     <row r="6" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="10" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="12" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="5">
-        <v>1</v>
-      </c>
-      <c r="G8" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="5">
-        <v>1.3</v>
-      </c>
-      <c r="G9" s="5">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="10" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="5">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G10" s="5">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="5">
+      <c r="F12" s="4">
+        <v>1.35</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="13" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="G13" s="4">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="14" spans="5:7" ht="28" x14ac:dyDescent="0.2">
+      <c r="E14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="4">
+        <v>1.35</v>
+      </c>
+      <c r="G14" s="4">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="15" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="7">
         <v>1.2</v>
       </c>
-      <c r="G11" s="5">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="12" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E12" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="5">
-        <v>1.35</v>
-      </c>
-      <c r="G12" s="5">
-        <v>1.35</v>
-      </c>
-    </row>
-    <row r="13" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E13" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="5">
-        <v>1.4</v>
-      </c>
-      <c r="G13" s="5">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="14" spans="5:7" ht="28" x14ac:dyDescent="0.2">
-      <c r="E14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="5">
-        <v>1.35</v>
-      </c>
-      <c r="G14" s="5">
-        <v>1.35</v>
-      </c>
-    </row>
-    <row r="15" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E15" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="8">
-        <v>1.2</v>
-      </c>
-      <c r="G15" s="8">
+      <c r="G15" s="7">
         <v>1.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Project Case412 is saved. master Type: SAVE.
</commit_message>
<xml_diff>
--- a/Case412/module1.xlsx
+++ b/Case412/module1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ekosolapova/work/bugs/TestCasesEPBDS-8483/Case4/Base/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ekosolapova/work/bugs/TestCasesEPBDS-8483/Case4/v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3440347A-CBCA-9846-BE8E-E203C3EC306C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078A9A76-1ACF-7545-AB36-3B5358099833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11980" yWindow="5900" windowWidth="27640" windowHeight="16940" xr2:uid="{D86F6ED2-5685-5F4F-AC05-266BA9A81085}"/>
   </bookViews>
@@ -84,9 +84,6 @@
     <t>OccasionallyOccupied</t>
   </si>
   <si>
-    <t xml:space="preserve">Other </t>
-  </si>
-  <si>
     <t>aaa</t>
   </si>
   <si>
@@ -94,6 +91,9 @@
   </si>
   <si>
     <t>SmartLookup Double Test ( String occupancyType, String policyForm )</t>
+  </si>
+  <si>
+    <t>Other 1</t>
   </si>
 </sst>
 </file>
@@ -202,9 +202,6 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -224,6 +221,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -544,7 +544,7 @@
   <dimension ref="E6:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -553,108 +553,108 @@
   </cols>
   <sheetData>
     <row r="6" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="10" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="12" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="4">
+        <v>1.35</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="13" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="G13" s="4">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="14" spans="5:7" ht="28" x14ac:dyDescent="0.2">
+      <c r="E14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="4">
+        <v>1.35</v>
+      </c>
+      <c r="G14" s="4">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="15" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E15" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="5">
-        <v>1</v>
-      </c>
-      <c r="G8" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="5">
-        <v>1.3</v>
-      </c>
-      <c r="G9" s="5">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="10" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="5">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G10" s="5">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="5">
+      <c r="F15" s="7">
         <v>1.2</v>
       </c>
-      <c r="G11" s="5">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="12" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E12" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="5">
-        <v>1.35</v>
-      </c>
-      <c r="G12" s="5">
-        <v>1.35</v>
-      </c>
-    </row>
-    <row r="13" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E13" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="5">
-        <v>1.4</v>
-      </c>
-      <c r="G13" s="5">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="14" spans="5:7" ht="28" x14ac:dyDescent="0.2">
-      <c r="E14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="5">
-        <v>1.35</v>
-      </c>
-      <c r="G14" s="5">
-        <v>1.35</v>
-      </c>
-    </row>
-    <row r="15" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E15" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="8">
-        <v>1.2</v>
-      </c>
-      <c r="G15" s="8">
+      <c r="G15" s="7">
         <v>1.2</v>
       </c>
     </row>

</xml_diff>